<commit_message>
Filled a couple time gaps in 2015 - all done now
</commit_message>
<xml_diff>
--- a/Q_issues_dec22.xlsx
+++ b/Q_issues_dec22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karen Jorgenson\Documents\Github\DoD_Discharge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE3F583-3EF4-4A42-BE9B-D5652110908B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7470EEFA-0549-48ED-82BB-FF210D472A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="735" windowWidth="17250" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="840" windowWidth="17250" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>Site</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Pressure data was below 100 (out of water) before 5/20</t>
+  </si>
+  <si>
+    <t>Raw data in 30 min intervals</t>
   </si>
 </sst>
 </file>
@@ -575,7 +578,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -679,6 +682,9 @@
       <c r="I4" t="s">
         <v>54</v>
       </c>
+      <c r="J4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -698,6 +704,9 @@
       </c>
       <c r="I5" t="s">
         <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>